<commit_message>
Mockup calendarizacion, actualizacion logt
</commit_message>
<xml_diff>
--- a/tspi/ciclo-3/20106065.xlsx
+++ b/tspi/ciclo-3/20106065.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400"/>
+    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Id</t>
   </si>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:ALY23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -17422,8 +17422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75"/>
@@ -17481,7 +17481,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="15">
-        <f t="shared" ref="F2:F6" si="0">((HOUR(D2)-HOUR(C2))*60)+(MINUTE(D2)-MINUTE(C2))-E2</f>
+        <f t="shared" ref="F2:F7" si="0">((HOUR(D2)-HOUR(C2))*60)+(MINUTE(D2)-MINUTE(C2))-E2</f>
         <v>27</v>
       </c>
       <c r="G2" s="20">
@@ -17597,11 +17597,31 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="26"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="26">
+        <v>41941</v>
+      </c>
+      <c r="B7" s="21">
+        <v>6</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.75694444444444453</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E7" s="21">
+        <v>0</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G7" s="20">
+        <v>49</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="26"/>

</xml_diff>